<commit_message>
creating files and section page based on excel spreadsheet
</commit_message>
<xml_diff>
--- a/sections.xlsx
+++ b/sections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Valculus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1944E549-E0D6-4177-AD9B-E596A1EA27CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EA4C17-4035-48A7-A562-4DC4A5DB0609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30000" windowHeight="17496" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30000" windowHeight="17496" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preliminaries" sheetId="1" r:id="rId1"/>
@@ -191,12 +191,6 @@
     <t>Areas of Polar Curves</t>
   </si>
   <si>
-    <t>Surface Area of Polar Curves</t>
-  </si>
-  <si>
-    <t>Conic Sections of Polar Functions</t>
-  </si>
-  <si>
     <t>Binomial Series</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t xml:space="preserve">Modeling of a particle moving along a parametric curve. Includes vector-valued functions: position, velocity, and acceleration. Discussion of speed and distance traveled. </t>
   </si>
   <si>
-    <t>Arclength of Polar Curves</t>
-  </si>
-  <si>
     <t>Introduction to polar coordinates. Conversion between polar and cartesian coordinates. Expression of polar functions as parametric functions of angle. Sketching polar graphs, with presentation of common graphs.</t>
   </si>
   <si>
@@ -492,6 +483,15 @@
   </si>
   <si>
     <t>Bounding the error when a partial sum is used to approximate an infinite series. Includes Alternating Series Bound, Taylor’s Remainder Theorem (Lagrange Error Bound), and remainders with the Integral Test.</t>
+  </si>
+  <si>
+    <t>Surface Area with Polar Curves</t>
+  </si>
+  <si>
+    <t>Arc Length of Polar Curves</t>
+  </si>
+  <si>
+    <t>Conic Sections with Polar Functions</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -873,7 +873,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -889,7 +889,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -899,10 +899,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,7 +916,7 @@
         <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -924,7 +924,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -932,35 +932,32 @@
         <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -969,10 +966,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,118 +980,115 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1120,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1128,7 +1122,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1136,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1144,7 +1138,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1152,7 +1146,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1160,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1168,7 +1162,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1204,7 +1198,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1212,7 +1206,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1220,7 +1214,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1228,7 +1222,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1236,7 +1230,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1244,7 +1238,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1271,7 +1265,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1279,7 +1273,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1287,7 +1281,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1295,7 +1289,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1303,7 +1297,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1311,7 +1305,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1319,7 +1313,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1327,7 +1321,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1351,10 +1345,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1362,7 +1356,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1370,7 +1364,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1378,7 +1372,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1386,7 +1380,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1407,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1421,31 +1415,31 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1453,7 +1447,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1461,7 +1455,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1469,7 +1463,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1477,15 +1471,15 @@
         <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1512,7 +1506,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1520,7 +1514,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1528,7 +1522,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1536,7 +1530,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1544,7 +1538,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1568,10 +1562,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1579,7 +1573,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1587,7 +1581,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1595,7 +1589,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1603,7 +1597,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1630,7 +1624,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1638,15 +1632,15 @@
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1654,7 +1648,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1662,7 +1656,7 @@
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>